<commit_message>
Signed-off-by: Mauricio Minella <mauriciominella@gmail.com>
</commit_message>
<xml_diff>
--- a/MoneyLoverDesktop/MoneyLoverDesktop/Excel/template/reportTemplate.xlsx
+++ b/MoneyLoverDesktop/MoneyLoverDesktop/Excel/template/reportTemplate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="8160" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="8160"/>
   </bookViews>
   <sheets>
     <sheet name="Despesas" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>Data</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Mês</t>
+  </si>
+  <si>
+    <t>Valor2</t>
   </si>
 </sst>
 </file>
@@ -119,9 +122,12 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
     <dxf>
       <numFmt numFmtId="166" formatCode="[$-416]mmmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -173,6 +179,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -197,7 +204,7 @@
           <c:explosion val="25"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Despesas por categoria'!$A$2:$A$14</c:f>
+              <c:f>'Despesas por categoria'!$A$2:$A$22</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -211,15 +218,116 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Despesas por categoria'!$B$2:$B$14</c:f>
+              <c:f>'Despesas por categoria'!$B$2:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Despesas por categoria'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Valor2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Despesas por categoria'!$A$2:$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Categoria 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Categoria 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Despesas por categoria'!$C$2:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -239,6 +347,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -289,8 +398,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:D56" insertRowShift="1" totalsRowShown="0">
-  <autoFilter ref="A1:D56"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:D3776" insertRowShift="1" totalsRowShown="0">
+  <autoFilter ref="A1:D3776"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Data"/>
     <tableColumn id="2" name="Categoria"/>
@@ -302,8 +411,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D13" insertRowShift="1" totalsRowShown="0">
-  <autoFilter ref="A1:D13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:D348" insertRowShift="1" totalsRowShown="0">
+  <autoFilter ref="A1:D348"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Data"/>
     <tableColumn id="2" name="Categoria"/>
@@ -315,11 +424,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:B14" totalsRowShown="0">
-  <autoFilter ref="A1:B14"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:C22" totalsRowShown="0">
+  <autoFilter ref="A1:C22"/>
+  <tableColumns count="3">
     <tableColumn id="1" name="Categoria"/>
-    <tableColumn id="2" name="Valor" dataDxfId="1"/>
+    <tableColumn id="2" name="Valor" dataDxfId="2"/>
+    <tableColumn id="3" name="Valor2" dataDxfId="1">
+      <calculatedColumnFormula>SUMIF(Table3[Categoria], Tabela1[[#This Row],[Categoria]], Table3[Valor])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -659,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D345"/>
   <sheetViews>
-    <sheetView topLeftCell="A380" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1726,8 +1838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A325" workbookViewId="0">
+      <selection activeCell="C333" sqref="C333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1759,10 +1871,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D218"/>
+  <dimension ref="A1:E218"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,90 +1883,177 @@
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="3">
+        <f>SUMIF(Table3[Categoria], Tabela1[[#This Row],[Categoria]], Table3[Valor])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="3">
+        <f>SUMIF(Table3[Categoria], Tabela1[[#This Row],[Categoria]], Table3[Valor])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="3">
+        <f>SUMIF(Table3[Categoria], Tabela1[[#This Row],[Categoria]], Table3[Valor])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="3">
+        <f>SUMIF(Table3[Categoria], Tabela1[[#This Row],[Categoria]], Table3[Valor])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="3">
+        <f>SUMIF(Table3[Categoria], Tabela1[[#This Row],[Categoria]], Table3[Valor])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="3">
+        <f>SUMIF(Table3[Categoria], Tabela1[[#This Row],[Categoria]], Table3[Valor])</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="3">
+        <f>SUMIF(Table3[Categoria], Tabela1[[#This Row],[Categoria]], Table3[Valor])</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="3">
+        <f>SUMIF(Table3[Categoria], Tabela1[[#This Row],[Categoria]], Table3[Valor])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="3">
+        <f>SUMIF(Table3[Categoria], Tabela1[[#This Row],[Categoria]], Table3[Valor])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="3">
+        <f>SUMIF(Table3[Categoria], Tabela1[[#This Row],[Categoria]], Table3[Valor])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="3">
+        <f>SUMIF(Table3[Categoria], Tabela1[[#This Row],[Categoria]], Table3[Valor])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="3">
+        <f>SUMIF(Table3[Categoria], Tabela1[[#This Row],[Categoria]], Table3[Valor])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="3">
+        <f>SUMIF(Table3[Categoria], Tabela1[[#This Row],[Categoria]], Table3[Valor])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="3">
+        <f>SUMIF(Table3[Categoria], Tabela1[[#This Row],[Categoria]], Table3[Valor])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
+      <c r="C16" s="3">
+        <f>SUMIF(Table3[Categoria], Tabela1[[#This Row],[Categoria]], Table3[Valor])</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
+      <c r="C17" s="3">
+        <f>SUMIF(Table3[Categoria], Tabela1[[#This Row],[Categoria]], Table3[Valor])</f>
+        <v>0</v>
+      </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
+      <c r="C18" s="3">
+        <f>SUMIF(Table3[Categoria], Tabela1[[#This Row],[Categoria]], Table3[Valor])</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
+      <c r="C19" s="3">
+        <f>SUMIF(Table3[Categoria], Tabela1[[#This Row],[Categoria]], Table3[Valor])</f>
+        <v>0</v>
+      </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
+      <c r="C20" s="3">
+        <f>SUMIF(Table3[Categoria], Tabela1[[#This Row],[Categoria]], Table3[Valor])</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
+      <c r="C21" s="3">
+        <f>SUMIF(Table3[Categoria], Tabela1[[#This Row],[Categoria]], Table3[Valor])</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
+      <c r="C22" s="3">
+        <f>SUMIF(Table3[Categoria], Tabela1[[#This Row],[Categoria]], Table3[Valor])</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
@@ -2522,7 +2721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>